<commit_message>
Create XlsxParser#letter_to_number XlsxParser#cell_value and related RSpec
</commit_message>
<xml_diff>
--- a/doc/xlsx_parser.xlsx
+++ b/doc/xlsx_parser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\ruby\xlsx2mysql\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF4CD37-8F84-4983-B38D-F5EDDFAF461B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467BC607-978D-46DF-8D0C-5F877A8CB1C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eudaimonia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C117</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L73</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BI110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,12 +389,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11580D06-7921-41B0-B2E7-C4075E5D8483}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AO86" workbookViewId="0">
+      <selection activeCell="BI110" sqref="BI110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="61:61" x14ac:dyDescent="0.25">
+      <c r="BI110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>